<commit_message>
Corrected the imputation code
</commit_message>
<xml_diff>
--- a/Shalomi_Updated.xlsx
+++ b/Shalomi_Updated.xlsx
@@ -969,9 +969,7 @@
       <c r="AF3" t="n">
         <v>5</v>
       </c>
-      <c r="AG3" t="n">
-        <v>4</v>
-      </c>
+      <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="n">
         <v>5</v>
       </c>
@@ -3319,9 +3317,7 @@
       <c r="AJ17" t="n">
         <v>1</v>
       </c>
-      <c r="AK17" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="n">
         <v>1</v>
       </c>
@@ -4989,9 +4985,7 @@
       <c r="AJ27" t="n">
         <v>0</v>
       </c>
-      <c r="AK27" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="n">
         <v>1</v>
       </c>
@@ -5490,9 +5484,7 @@
       <c r="AJ30" t="n">
         <v>0</v>
       </c>
-      <c r="AK30" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK30" t="inlineStr"/>
       <c r="AL30" t="n">
         <v>1</v>
       </c>
@@ -5657,9 +5649,7 @@
       <c r="AJ31" t="n">
         <v>0</v>
       </c>
-      <c r="AK31" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK31" t="inlineStr"/>
       <c r="AL31" t="n">
         <v>1</v>
       </c>
@@ -6492,9 +6482,7 @@
       <c r="AJ36" t="n">
         <v>0</v>
       </c>
-      <c r="AK36" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK36" t="inlineStr"/>
       <c r="AL36" t="n">
         <v>1</v>
       </c>
@@ -6659,9 +6647,7 @@
       <c r="AJ37" t="n">
         <v>1</v>
       </c>
-      <c r="AK37" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK37" t="inlineStr"/>
       <c r="AL37" t="n">
         <v>1</v>
       </c>
@@ -11827,9 +11813,7 @@
       <c r="AG68" t="n">
         <v>4</v>
       </c>
-      <c r="AH68" t="n">
-        <v>5</v>
-      </c>
+      <c r="AH68" t="inlineStr"/>
       <c r="AI68" t="n">
         <v>3</v>
       </c>
@@ -14165,9 +14149,7 @@
       <c r="AG82" t="n">
         <v>4</v>
       </c>
-      <c r="AH82" t="n">
-        <v>5</v>
-      </c>
+      <c r="AH82" t="inlineStr"/>
       <c r="AI82" t="n">
         <v>4</v>
       </c>
@@ -14332,9 +14314,7 @@
       <c r="AG83" t="n">
         <v>3</v>
       </c>
-      <c r="AH83" t="n">
-        <v>5</v>
-      </c>
+      <c r="AH83" t="inlineStr"/>
       <c r="AI83" t="n">
         <v>3</v>
       </c>
@@ -15000,9 +14980,7 @@
       <c r="AG87" t="n">
         <v>4</v>
       </c>
-      <c r="AH87" t="n">
-        <v>5</v>
-      </c>
+      <c r="AH87" t="inlineStr"/>
       <c r="AI87" t="n">
         <v>5</v>
       </c>

</xml_diff>